<commit_message>
multi implemented CRargs not working
</commit_message>
<xml_diff>
--- a/info/ADT.xlsx
+++ b/info/ADT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/Dropbox/Icke/Work/SequencingOrga/scRNA-seq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/Sites/Bio/cellrangersnake/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC2A27-A0E1-D647-A1FE-CE6BADB91FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809FBC5C-2721-3D4B-A03D-89D7DBAB34D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="760" windowWidth="15060" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="760" windowWidth="15060" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="211001" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="220302" sheetId="3" r:id="rId3"/>
     <sheet name="221004" sheetId="5" r:id="rId4"/>
     <sheet name="221018" sheetId="4" r:id="rId5"/>
+    <sheet name="230114" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3899" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4801" uniqueCount="943">
   <si>
     <t>Gene</t>
   </si>
@@ -14972,8 +14973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206BAB6A-9683-684F-983B-EADF05D11963}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18471,4 +18472,3512 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5EB16E-FEFA-B04B-891D-015DF455A8BB}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:I145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>838</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>839</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>840</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
+        <v>841</v>
+      </c>
+      <c r="F4" s="1">
+        <v>122</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>842</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>843</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>844</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" t="s">
+        <v>937</v>
+      </c>
+      <c r="D19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" t="s">
+        <v>845</v>
+      </c>
+      <c r="C24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C29" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" t="s">
+        <v>229</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" t="s">
+        <v>938</v>
+      </c>
+      <c r="D30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" t="s">
+        <v>235</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B32" t="s">
+        <v>846</v>
+      </c>
+      <c r="C32" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" t="s">
+        <v>847</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C33" t="s">
+        <v>918</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" t="s">
+        <v>246</v>
+      </c>
+      <c r="C34" t="s">
+        <v>919</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" t="s">
+        <v>920</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36" t="s">
+        <v>254</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" t="s">
+        <v>260</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" t="s">
+        <v>848</v>
+      </c>
+      <c r="C38" t="s">
+        <v>264</v>
+      </c>
+      <c r="D38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E38" t="s">
+        <v>849</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B39" t="s">
+        <v>269</v>
+      </c>
+      <c r="C39" t="s">
+        <v>270</v>
+      </c>
+      <c r="D39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" t="s">
+        <v>274</v>
+      </c>
+      <c r="D40" t="s">
+        <v>275</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" t="s">
+        <v>280</v>
+      </c>
+      <c r="D41" t="s">
+        <v>281</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H41" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" t="s">
+        <v>286</v>
+      </c>
+      <c r="D42" t="s">
+        <v>287</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H42" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B43" t="s">
+        <v>850</v>
+      </c>
+      <c r="C43" t="s">
+        <v>291</v>
+      </c>
+      <c r="D43" t="s">
+        <v>292</v>
+      </c>
+      <c r="E43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" t="s">
+        <v>851</v>
+      </c>
+      <c r="C44" t="s">
+        <v>294</v>
+      </c>
+      <c r="D44" t="s">
+        <v>295</v>
+      </c>
+      <c r="E44" t="s">
+        <v>294</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B45" t="s">
+        <v>297</v>
+      </c>
+      <c r="C45" t="s">
+        <v>298</v>
+      </c>
+      <c r="D45" t="s">
+        <v>299</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H45" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B46" t="s">
+        <v>852</v>
+      </c>
+      <c r="C46" t="s">
+        <v>303</v>
+      </c>
+      <c r="D46" t="s">
+        <v>304</v>
+      </c>
+      <c r="E46" t="s">
+        <v>303</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B47" t="s">
+        <v>853</v>
+      </c>
+      <c r="C47" t="s">
+        <v>308</v>
+      </c>
+      <c r="D47" t="s">
+        <v>309</v>
+      </c>
+      <c r="E47" t="s">
+        <v>308</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B48" t="s">
+        <v>854</v>
+      </c>
+      <c r="C48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D48" t="s">
+        <v>312</v>
+      </c>
+      <c r="E48" t="s">
+        <v>855</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H48" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B49" t="s">
+        <v>316</v>
+      </c>
+      <c r="C49" t="s">
+        <v>317</v>
+      </c>
+      <c r="D49" t="s">
+        <v>318</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B50" t="s">
+        <v>320</v>
+      </c>
+      <c r="C50" t="s">
+        <v>321</v>
+      </c>
+      <c r="D50" t="s">
+        <v>322</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B51" t="s">
+        <v>326</v>
+      </c>
+      <c r="C51" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" t="s">
+        <v>328</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="H51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B52" t="s">
+        <v>856</v>
+      </c>
+      <c r="C52" t="s">
+        <v>332</v>
+      </c>
+      <c r="D52" t="s">
+        <v>333</v>
+      </c>
+      <c r="E52" t="s">
+        <v>826</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B53" t="s">
+        <v>857</v>
+      </c>
+      <c r="C53" t="s">
+        <v>335</v>
+      </c>
+      <c r="D53" t="s">
+        <v>336</v>
+      </c>
+      <c r="E53" t="s">
+        <v>858</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="H53" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B54" t="s">
+        <v>859</v>
+      </c>
+      <c r="C54" t="s">
+        <v>340</v>
+      </c>
+      <c r="D54" t="s">
+        <v>341</v>
+      </c>
+      <c r="E54" t="s">
+        <v>860</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" t="s">
+        <v>345</v>
+      </c>
+      <c r="C55" t="s">
+        <v>346</v>
+      </c>
+      <c r="D55" t="s">
+        <v>347</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" t="s">
+        <v>861</v>
+      </c>
+      <c r="C56" t="s">
+        <v>349</v>
+      </c>
+      <c r="D56" t="s">
+        <v>350</v>
+      </c>
+      <c r="E56" t="s">
+        <v>862</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H56" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B57" t="s">
+        <v>863</v>
+      </c>
+      <c r="C57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D57" t="s">
+        <v>355</v>
+      </c>
+      <c r="E57" t="s">
+        <v>820</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H57" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B58" t="s">
+        <v>864</v>
+      </c>
+      <c r="C58" t="s">
+        <v>357</v>
+      </c>
+      <c r="D58" t="s">
+        <v>358</v>
+      </c>
+      <c r="E58" t="s">
+        <v>865</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="H58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B59" t="s">
+        <v>362</v>
+      </c>
+      <c r="C59" t="s">
+        <v>363</v>
+      </c>
+      <c r="D59" t="s">
+        <v>364</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B60" t="s">
+        <v>366</v>
+      </c>
+      <c r="C60" t="s">
+        <v>367</v>
+      </c>
+      <c r="D60" t="s">
+        <v>368</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="H60" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B61" t="s">
+        <v>372</v>
+      </c>
+      <c r="C61" t="s">
+        <v>373</v>
+      </c>
+      <c r="D61" t="s">
+        <v>374</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H61" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B62" t="s">
+        <v>378</v>
+      </c>
+      <c r="C62" t="s">
+        <v>379</v>
+      </c>
+      <c r="D62" t="s">
+        <v>380</v>
+      </c>
+      <c r="F62" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="H62" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B63" t="s">
+        <v>866</v>
+      </c>
+      <c r="C63" t="s">
+        <v>383</v>
+      </c>
+      <c r="D63" t="s">
+        <v>384</v>
+      </c>
+      <c r="E63" t="s">
+        <v>867</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="H63" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B64" t="s">
+        <v>388</v>
+      </c>
+      <c r="C64" t="s">
+        <v>389</v>
+      </c>
+      <c r="D64" t="s">
+        <v>390</v>
+      </c>
+      <c r="F64" s="1">
+        <v>51.1</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H64" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B65" t="s">
+        <v>868</v>
+      </c>
+      <c r="C65" t="s">
+        <v>393</v>
+      </c>
+      <c r="D65" t="s">
+        <v>394</v>
+      </c>
+      <c r="E65" t="s">
+        <v>869</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="H65" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B66" t="s">
+        <v>398</v>
+      </c>
+      <c r="C66" t="s">
+        <v>399</v>
+      </c>
+      <c r="D66" t="s">
+        <v>400</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="H66" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B67" t="s">
+        <v>404</v>
+      </c>
+      <c r="C67" t="s">
+        <v>405</v>
+      </c>
+      <c r="D67" t="s">
+        <v>406</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="H67" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B68" t="s">
+        <v>870</v>
+      </c>
+      <c r="C68" t="s">
+        <v>410</v>
+      </c>
+      <c r="D68" t="s">
+        <v>411</v>
+      </c>
+      <c r="E68" t="s">
+        <v>410</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="H68" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B69" t="s">
+        <v>871</v>
+      </c>
+      <c r="C69" t="s">
+        <v>415</v>
+      </c>
+      <c r="D69" t="s">
+        <v>416</v>
+      </c>
+      <c r="E69" t="s">
+        <v>415</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="H69" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B70" t="s">
+        <v>872</v>
+      </c>
+      <c r="C70" t="s">
+        <v>420</v>
+      </c>
+      <c r="D70" t="s">
+        <v>421</v>
+      </c>
+      <c r="E70" t="s">
+        <v>816</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H70" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B71" t="s">
+        <v>423</v>
+      </c>
+      <c r="C71" t="s">
+        <v>424</v>
+      </c>
+      <c r="D71" t="s">
+        <v>425</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B72" t="s">
+        <v>427</v>
+      </c>
+      <c r="C72" t="s">
+        <v>428</v>
+      </c>
+      <c r="D72" t="s">
+        <v>429</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="H72" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B73" t="s">
+        <v>433</v>
+      </c>
+      <c r="C73" t="s">
+        <v>434</v>
+      </c>
+      <c r="D73" t="s">
+        <v>435</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="H73" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B74" t="s">
+        <v>439</v>
+      </c>
+      <c r="C74" t="s">
+        <v>440</v>
+      </c>
+      <c r="D74" t="s">
+        <v>441</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H74" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B75" t="s">
+        <v>445</v>
+      </c>
+      <c r="C75" t="s">
+        <v>446</v>
+      </c>
+      <c r="D75" t="s">
+        <v>447</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B76" t="s">
+        <v>873</v>
+      </c>
+      <c r="C76" t="s">
+        <v>449</v>
+      </c>
+      <c r="D76" t="s">
+        <v>450</v>
+      </c>
+      <c r="E76" t="s">
+        <v>874</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="H76" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B77" t="s">
+        <v>875</v>
+      </c>
+      <c r="C77" t="s">
+        <v>454</v>
+      </c>
+      <c r="D77" t="s">
+        <v>455</v>
+      </c>
+      <c r="E77" t="s">
+        <v>876</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="H77" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B78" t="s">
+        <v>877</v>
+      </c>
+      <c r="C78" t="s">
+        <v>459</v>
+      </c>
+      <c r="D78" t="s">
+        <v>460</v>
+      </c>
+      <c r="E78" t="s">
+        <v>878</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="H78" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B79" t="s">
+        <v>464</v>
+      </c>
+      <c r="C79" t="s">
+        <v>465</v>
+      </c>
+      <c r="D79" t="s">
+        <v>466</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="H79" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B80" t="s">
+        <v>879</v>
+      </c>
+      <c r="C80" t="s">
+        <v>470</v>
+      </c>
+      <c r="D80" t="s">
+        <v>471</v>
+      </c>
+      <c r="E80" t="s">
+        <v>880</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="H80" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B81" t="s">
+        <v>475</v>
+      </c>
+      <c r="C81" t="s">
+        <v>476</v>
+      </c>
+      <c r="D81" t="s">
+        <v>477</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="H81" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B82" t="s">
+        <v>481</v>
+      </c>
+      <c r="C82" t="s">
+        <v>482</v>
+      </c>
+      <c r="D82" t="s">
+        <v>483</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="H82" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B83" t="s">
+        <v>881</v>
+      </c>
+      <c r="C83" t="s">
+        <v>487</v>
+      </c>
+      <c r="D83" t="s">
+        <v>488</v>
+      </c>
+      <c r="E83" t="s">
+        <v>882</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="H83" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B84" t="s">
+        <v>883</v>
+      </c>
+      <c r="C84" t="s">
+        <v>492</v>
+      </c>
+      <c r="D84" t="s">
+        <v>493</v>
+      </c>
+      <c r="E84" t="s">
+        <v>884</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="H84" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B85" t="s">
+        <v>497</v>
+      </c>
+      <c r="C85" t="s">
+        <v>923</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="H85" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B86" t="s">
+        <v>501</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>924</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="H86" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B87" t="s">
+        <v>505</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>921</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="H87" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B88" t="s">
+        <v>509</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>925</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="H88" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B89" t="s">
+        <v>885</v>
+      </c>
+      <c r="C89" t="s">
+        <v>513</v>
+      </c>
+      <c r="D89" t="s">
+        <v>514</v>
+      </c>
+      <c r="E89" t="s">
+        <v>886</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H89" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B90" t="s">
+        <v>887</v>
+      </c>
+      <c r="C90" t="s">
+        <v>518</v>
+      </c>
+      <c r="D90" t="s">
+        <v>519</v>
+      </c>
+      <c r="E90" t="s">
+        <v>888</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="H90" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B91" t="s">
+        <v>523</v>
+      </c>
+      <c r="C91" t="s">
+        <v>524</v>
+      </c>
+      <c r="D91" t="s">
+        <v>525</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="H91" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B92" t="s">
+        <v>529</v>
+      </c>
+      <c r="C92" t="s">
+        <v>530</v>
+      </c>
+      <c r="D92" t="s">
+        <v>531</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="H92" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B93" t="s">
+        <v>889</v>
+      </c>
+      <c r="C93" t="s">
+        <v>535</v>
+      </c>
+      <c r="D93" t="s">
+        <v>536</v>
+      </c>
+      <c r="E93" t="s">
+        <v>824</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H93" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B94" t="s">
+        <v>538</v>
+      </c>
+      <c r="C94" t="s">
+        <v>539</v>
+      </c>
+      <c r="D94" t="s">
+        <v>540</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="H94" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B95" t="s">
+        <v>544</v>
+      </c>
+      <c r="C95" t="s">
+        <v>545</v>
+      </c>
+      <c r="D95" t="s">
+        <v>546</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="H95" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B96" t="s">
+        <v>890</v>
+      </c>
+      <c r="C96" t="s">
+        <v>550</v>
+      </c>
+      <c r="D96" t="s">
+        <v>551</v>
+      </c>
+      <c r="E96" t="s">
+        <v>891</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="H96" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B97" t="s">
+        <v>555</v>
+      </c>
+      <c r="C97" t="s">
+        <v>556</v>
+      </c>
+      <c r="D97" t="s">
+        <v>557</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="H97" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B98" t="s">
+        <v>561</v>
+      </c>
+      <c r="C98" t="s">
+        <v>562</v>
+      </c>
+      <c r="D98" t="s">
+        <v>563</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="H98" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B99" t="s">
+        <v>892</v>
+      </c>
+      <c r="C99" t="s">
+        <v>567</v>
+      </c>
+      <c r="D99" t="s">
+        <v>568</v>
+      </c>
+      <c r="E99" t="s">
+        <v>893</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="H99" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B100" t="s">
+        <v>572</v>
+      </c>
+      <c r="C100" t="s">
+        <v>573</v>
+      </c>
+      <c r="D100" t="s">
+        <v>574</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="H100" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B101" t="s">
+        <v>894</v>
+      </c>
+      <c r="C101" t="s">
+        <v>578</v>
+      </c>
+      <c r="D101" t="s">
+        <v>579</v>
+      </c>
+      <c r="E101" t="s">
+        <v>895</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="H101" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B102" t="s">
+        <v>583</v>
+      </c>
+      <c r="C102" t="s">
+        <v>584</v>
+      </c>
+      <c r="D102" t="s">
+        <v>585</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="H102" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B103" t="s">
+        <v>896</v>
+      </c>
+      <c r="C103" t="s">
+        <v>589</v>
+      </c>
+      <c r="D103" t="s">
+        <v>590</v>
+      </c>
+      <c r="E103" t="s">
+        <v>897</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="H103" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B104" t="s">
+        <v>594</v>
+      </c>
+      <c r="C104" t="s">
+        <v>595</v>
+      </c>
+      <c r="D104" t="s">
+        <v>596</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="H104" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B105" t="s">
+        <v>600</v>
+      </c>
+      <c r="C105" t="s">
+        <v>601</v>
+      </c>
+      <c r="D105" t="s">
+        <v>602</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="H105" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B106" t="s">
+        <v>606</v>
+      </c>
+      <c r="C106" t="s">
+        <v>607</v>
+      </c>
+      <c r="D106" t="s">
+        <v>608</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H106" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B107" t="s">
+        <v>610</v>
+      </c>
+      <c r="C107" t="s">
+        <v>611</v>
+      </c>
+      <c r="D107" t="s">
+        <v>612</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="H107" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B108" t="s">
+        <v>898</v>
+      </c>
+      <c r="C108" t="s">
+        <v>616</v>
+      </c>
+      <c r="D108" t="s">
+        <v>617</v>
+      </c>
+      <c r="E108" t="s">
+        <v>822</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H108" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B109" t="s">
+        <v>619</v>
+      </c>
+      <c r="C109" t="s">
+        <v>939</v>
+      </c>
+      <c r="D109" t="s">
+        <v>174</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="H109" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B110" t="s">
+        <v>623</v>
+      </c>
+      <c r="C110" t="s">
+        <v>624</v>
+      </c>
+      <c r="D110" t="s">
+        <v>625</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="H110" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B111" t="s">
+        <v>629</v>
+      </c>
+      <c r="C111" t="s">
+        <v>630</v>
+      </c>
+      <c r="D111" t="s">
+        <v>631</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="H111" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B112" t="s">
+        <v>635</v>
+      </c>
+      <c r="C112" t="s">
+        <v>636</v>
+      </c>
+      <c r="D112" t="s">
+        <v>637</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="H112" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B113" t="s">
+        <v>641</v>
+      </c>
+      <c r="C113" t="s">
+        <v>642</v>
+      </c>
+      <c r="D113" t="s">
+        <v>643</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="H113" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B114" t="s">
+        <v>899</v>
+      </c>
+      <c r="C114" t="s">
+        <v>647</v>
+      </c>
+      <c r="D114" t="s">
+        <v>648</v>
+      </c>
+      <c r="E114" t="s">
+        <v>900</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="H114" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B115" t="s">
+        <v>652</v>
+      </c>
+      <c r="C115" t="s">
+        <v>653</v>
+      </c>
+      <c r="D115" t="s">
+        <v>654</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="H115" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B116" t="s">
+        <v>658</v>
+      </c>
+      <c r="C116" t="s">
+        <v>659</v>
+      </c>
+      <c r="D116" t="s">
+        <v>660</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H116" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B117" t="s">
+        <v>901</v>
+      </c>
+      <c r="C117" t="s">
+        <v>662</v>
+      </c>
+      <c r="D117" t="s">
+        <v>663</v>
+      </c>
+      <c r="E117" t="s">
+        <v>818</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H117" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B118" t="s">
+        <v>665</v>
+      </c>
+      <c r="C118" t="s">
+        <v>926</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="H118" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B119" t="s">
+        <v>669</v>
+      </c>
+      <c r="C119" t="s">
+        <v>927</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H119" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B120" t="s">
+        <v>673</v>
+      </c>
+      <c r="C120" t="s">
+        <v>674</v>
+      </c>
+      <c r="D120" t="s">
+        <v>675</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="H120" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B121" t="s">
+        <v>902</v>
+      </c>
+      <c r="C121" t="s">
+        <v>679</v>
+      </c>
+      <c r="D121" t="s">
+        <v>680</v>
+      </c>
+      <c r="E121" t="s">
+        <v>903</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="H121" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B122" t="s">
+        <v>904</v>
+      </c>
+      <c r="C122" t="s">
+        <v>684</v>
+      </c>
+      <c r="D122" t="s">
+        <v>685</v>
+      </c>
+      <c r="E122" t="s">
+        <v>905</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H122" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B123" t="s">
+        <v>906</v>
+      </c>
+      <c r="C123" t="s">
+        <v>689</v>
+      </c>
+      <c r="D123" t="s">
+        <v>690</v>
+      </c>
+      <c r="E123" t="s">
+        <v>907</v>
+      </c>
+      <c r="F123" s="1">
+        <v>162.1</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="H123" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B124" t="s">
+        <v>693</v>
+      </c>
+      <c r="C124" t="s">
+        <v>694</v>
+      </c>
+      <c r="D124" t="s">
+        <v>695</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H124" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B125" t="s">
+        <v>699</v>
+      </c>
+      <c r="C125" t="s">
+        <v>700</v>
+      </c>
+      <c r="D125" t="s">
+        <v>701</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="H125" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B126" t="s">
+        <v>908</v>
+      </c>
+      <c r="C126" t="s">
+        <v>705</v>
+      </c>
+      <c r="D126" t="s">
+        <v>706</v>
+      </c>
+      <c r="E126" t="s">
+        <v>909</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="H126" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B127" t="s">
+        <v>710</v>
+      </c>
+      <c r="C127" t="s">
+        <v>711</v>
+      </c>
+      <c r="D127" t="s">
+        <v>712</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="H127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B128" t="s">
+        <v>716</v>
+      </c>
+      <c r="C128" t="s">
+        <v>942</v>
+      </c>
+      <c r="D128" t="s">
+        <v>718</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="H128" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B129" t="s">
+        <v>910</v>
+      </c>
+      <c r="C129" t="s">
+        <v>722</v>
+      </c>
+      <c r="D129" t="s">
+        <v>723</v>
+      </c>
+      <c r="E129" t="s">
+        <v>911</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="H129" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B130" t="s">
+        <v>727</v>
+      </c>
+      <c r="C130" t="s">
+        <v>728</v>
+      </c>
+      <c r="D130" t="s">
+        <v>729</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="H130" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B131" t="s">
+        <v>733</v>
+      </c>
+      <c r="C131" t="s">
+        <v>941</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="H131" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B132" t="s">
+        <v>912</v>
+      </c>
+      <c r="C132" t="s">
+        <v>737</v>
+      </c>
+      <c r="D132" t="s">
+        <v>738</v>
+      </c>
+      <c r="E132" t="s">
+        <v>913</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="H132" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B133" t="s">
+        <v>742</v>
+      </c>
+      <c r="C133" t="s">
+        <v>743</v>
+      </c>
+      <c r="D133" t="s">
+        <v>744</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="H133" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B134" t="s">
+        <v>748</v>
+      </c>
+      <c r="C134" t="s">
+        <v>749</v>
+      </c>
+      <c r="D134" t="s">
+        <v>750</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="H134" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B135" t="s">
+        <v>754</v>
+      </c>
+      <c r="C135" t="s">
+        <v>755</v>
+      </c>
+      <c r="D135" t="s">
+        <v>756</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="H135" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B136" t="s">
+        <v>914</v>
+      </c>
+      <c r="C136" t="s">
+        <v>760</v>
+      </c>
+      <c r="D136" t="s">
+        <v>761</v>
+      </c>
+      <c r="E136" t="s">
+        <v>762</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="H136" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B137" t="s">
+        <v>915</v>
+      </c>
+      <c r="C137" t="s">
+        <v>765</v>
+      </c>
+      <c r="D137" t="s">
+        <v>766</v>
+      </c>
+      <c r="E137" t="s">
+        <v>916</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="H137" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B138" t="s">
+        <v>770</v>
+      </c>
+      <c r="C138" t="s">
+        <v>771</v>
+      </c>
+      <c r="D138" t="s">
+        <v>772</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="H138" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B139" t="s">
+        <v>776</v>
+      </c>
+      <c r="C139" t="s">
+        <v>917</v>
+      </c>
+      <c r="D139" t="s">
+        <v>777</v>
+      </c>
+      <c r="F139" t="s">
+        <v>778</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="H139" s="10">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B140" t="s">
+        <v>781</v>
+      </c>
+      <c r="C140" t="s">
+        <v>782</v>
+      </c>
+      <c r="D140" t="s">
+        <v>783</v>
+      </c>
+      <c r="F140" t="s">
+        <v>784</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="H140" s="10">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B141" t="s">
+        <v>787</v>
+      </c>
+      <c r="C141" t="s">
+        <v>788</v>
+      </c>
+      <c r="D141" t="s">
+        <v>789</v>
+      </c>
+      <c r="F141" t="s">
+        <v>790</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="H141" s="10">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B142" t="s">
+        <v>793</v>
+      </c>
+      <c r="C142" t="s">
+        <v>794</v>
+      </c>
+      <c r="D142" t="s">
+        <v>795</v>
+      </c>
+      <c r="F142" t="s">
+        <v>796</v>
+      </c>
+      <c r="G142" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="H142" s="10">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B143" t="s">
+        <v>799</v>
+      </c>
+      <c r="C143" t="s">
+        <v>928</v>
+      </c>
+      <c r="F143" t="s">
+        <v>69</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H143" s="10">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B144" t="s">
+        <v>801</v>
+      </c>
+      <c r="C144" t="s">
+        <v>929</v>
+      </c>
+      <c r="F144" t="s">
+        <v>69</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H144" s="10">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B145" t="s">
+        <v>803</v>
+      </c>
+      <c r="C145" t="s">
+        <v>930</v>
+      </c>
+      <c r="F145" t="s">
+        <v>69</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H145" s="10">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{5F49A109-3B12-D146-B4B4-A645B1FFFD34}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H2:H145</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>